<commit_message>
Forcefully removed TSLA_stock_data_horizontal.xlsx from repository
</commit_message>
<xml_diff>
--- a/TSLA_stock_data.xlsx
+++ b/TSLA_stock_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,166 +439,200 @@
           <t>Stock Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B2" t="n">
+        <v>262.67</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Change</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="B3" t="n">
+        <v>-0.7799988</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Previous Close</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="B4" t="n">
+        <v>263.45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Open</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="B5" t="n">
+        <v>259.275</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Bid</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="B6" t="n">
+        <v>262.23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Ask</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="B7" t="n">
+        <v>272.52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Day's Range</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>250.73 - 266.2499</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>52 Week Range</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>138.8 - 488.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="B10" t="n">
+        <v>101496505</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Avg. Volume</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="B11" t="n">
+        <v>86384041</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Market Cap</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="B12" t="n">
+        <v>844883361792</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="B13" t="n">
+        <v>2.507</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>PE Ratio (TTM)</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="B14" t="n">
+        <v>128.13171</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>EPS</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="B15" t="n">
+        <v>2.05</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Earnings Date</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>Forward Dividend &amp; Yield</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Ex-Dividend Date</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>1y Target Est</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tesla, Inc.</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>279.1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>7.0599976</v>
-      </c>
-      <c r="D2" t="n">
-        <v>272.04</v>
-      </c>
-      <c r="E2" t="n">
-        <v>272.96</v>
-      </c>
-      <c r="F2" t="n">
-        <v>278.87</v>
-      </c>
-      <c r="G2" t="n">
-        <v>279.23</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>267.71 - 279.54</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>138.8 - 488.54</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>93248500</v>
-      </c>
-      <c r="K2" t="n">
-        <v>85678636</v>
-      </c>
-      <c r="L2" t="n">
-        <v>897730740224</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2.507</v>
-      </c>
-      <c r="N2" t="n">
-        <v>136.81374</v>
-      </c>
-      <c r="O2" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>342.3445</v>
+      <c r="B19" t="n">
+        <v>345.63025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>